<commit_message>
Excel sheet has been imported with keepers.
Co-authored-by: Mitch V Aureli  <mitchellaha@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Top 300.xlsx
+++ b/Top 300.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cammy Sabby\Documents\Fantasy Baseball\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu20.04LTS\home\cammysabby\Repositories\DraftBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2661F6-B5DB-4091-95A3-A8156CC74900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D601F49E-E06A-42C2-BF93-14652337C9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2432445B-5839-490F-84C0-08243701B289}"/>
+    <workbookView xWindow="6840" yWindow="1650" windowWidth="28800" windowHeight="15345" xr2:uid="{2432445B-5839-490F-84C0-08243701B289}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -771,10 +771,10 @@
     <t>SP</t>
   </si>
   <si>
-    <t>Positions</t>
-  </si>
-  <si>
     <t>Player Name</t>
+  </si>
+  <si>
+    <t>Position</t>
   </si>
 </sst>
 </file>
@@ -1140,7 +1140,7 @@
   <dimension ref="A1:C299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,13 +1152,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
         <v>237</v>
       </c>
       <c r="C1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4172,21 +4172,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003B265D840FD628468CE89AE87D2C74EF" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e6ada9ba706a31a2c9eb63edacf7ecd0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9e05df9f-ab78-451b-9021-920a7657ab04" xmlns:ns4="ff44e8c4-adf4-45f7-97b6-9eed51ba971e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0be3cb3b0aa890b837a2415d4214c4a" ns3:_="" ns4:_="">
     <xsd:import namespace="9e05df9f-ab78-451b-9021-920a7657ab04"/>
@@ -4371,32 +4356,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C157DD8-8F72-44B5-A288-D5608592A50F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ff44e8c4-adf4-45f7-97b6-9eed51ba971e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="9e05df9f-ab78-451b-9021-920a7657ab04"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C365D580-1C5C-4C17-9DF1-E479F4326582}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B996D1A0-D94F-4658-B738-DEAC12FACD01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4413,4 +4388,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C365D580-1C5C-4C17-9DF1-E479F4326582}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C157DD8-8F72-44B5-A288-D5608592A50F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ff44e8c4-adf4-45f7-97b6-9eed51ba971e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="9e05df9f-ab78-451b-9021-920a7657ab04"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>